<commit_message>
create batch windows file
</commit_message>
<xml_diff>
--- a/software/resultados_ciclogen.xlsx
+++ b/software/resultados_ciclogen.xlsx
@@ -413,19 +413,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>254.45</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>530</v>
+        <v>320</v>
       </c>
       <c r="D2" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E2" t="n">
-        <v>3488.97239332325</v>
+        <v>3065.056341566094</v>
       </c>
       <c r="F2" t="n">
-        <v>6.930924188546035</v>
+        <v>6.796725879902986</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -443,19 +443,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>254.45</v>
+        <v>221.5</v>
       </c>
       <c r="C3" t="n">
-        <v>530</v>
+        <v>320</v>
       </c>
       <c r="D3" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E3" t="n">
-        <v>3488.97239332325</v>
+        <v>3065.056341566094</v>
       </c>
       <c r="F3" t="n">
-        <v>6.930924188546035</v>
+        <v>6.796725879902986</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -473,19 +473,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>254.45</v>
+        <v>221.5</v>
       </c>
       <c r="C4" t="n">
-        <v>182.217146973062</v>
+        <v>174.8941768640577</v>
       </c>
       <c r="D4" t="n">
         <v>2.5</v>
       </c>
       <c r="E4" t="n">
-        <v>2832.043502651045</v>
+        <v>2817.006492904334</v>
       </c>
       <c r="F4" t="n">
-        <v>7.323045272477203</v>
+        <v>7.289754939244287</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -503,19 +503,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>116.28365</v>
+        <v>28.50000000000002</v>
       </c>
       <c r="C5" t="n">
-        <v>182.217146973062</v>
+        <v>319.9999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>2.5</v>
+        <v>22</v>
       </c>
       <c r="E5" t="n">
-        <v>2832.043502651045</v>
+        <v>3065.056341566094</v>
       </c>
       <c r="F5" t="n">
-        <v>7.323045272477203</v>
+        <v>6.796725879902986</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -533,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>116.28365</v>
+        <v>28.50000000000002</v>
       </c>
       <c r="C6" t="n">
         <v>41.50876547963827</v>
@@ -542,10 +542,10 @@
         <v>0.08</v>
       </c>
       <c r="E6" t="n">
-        <v>2399.74282027538</v>
+        <v>2313.856579806076</v>
       </c>
       <c r="F6" t="n">
-        <v>7.66651312543588</v>
+        <v>7.393562710918144</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>92.65462087336374</v>
+        <v>89.07955179903253</v>
       </c>
     </row>
     <row r="7">
@@ -561,7 +561,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>116.28365</v>
+        <v>28.50000000000002</v>
       </c>
       <c r="C7" t="n">
         <v>41.50876547963827</v>
@@ -570,7 +570,7 @@
         <v>0.08</v>
       </c>
       <c r="E7" t="n">
-        <v>173.8398003706382</v>
+        <v>173.8398003706387</v>
       </c>
       <c r="F7" t="n">
         <v>0.5924911559165427</v>
@@ -589,19 +589,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>116.28365</v>
+        <v>28.50000000000002</v>
       </c>
       <c r="C8" t="n">
-        <v>41.53552743030059</v>
+        <v>41.53552743031628</v>
       </c>
       <c r="D8" t="n">
         <v>2.5</v>
       </c>
       <c r="E8" t="n">
-        <v>174.1652036954723</v>
+        <v>174.1652036954729</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5927497189589911</v>
+        <v>0.5927497189592826</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -619,19 +619,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>108.434503625</v>
+        <v>19.00950000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>41.53552743030059</v>
+        <v>41.53552743031628</v>
       </c>
       <c r="D9" t="n">
         <v>2.5</v>
       </c>
       <c r="E9" t="n">
-        <v>174.1652036954723</v>
+        <v>174.1652036954729</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5927497189589911</v>
+        <v>0.5927497189592826</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -649,19 +649,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>7.849146375000002</v>
+        <v>9.490500000000004</v>
       </c>
       <c r="C10" t="n">
-        <v>41.53552743030059</v>
+        <v>41.53552743031628</v>
       </c>
       <c r="D10" t="n">
         <v>2.5</v>
       </c>
       <c r="E10" t="n">
-        <v>174.1652036954723</v>
+        <v>174.1652036954729</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5927497189589911</v>
+        <v>0.5927497189592826</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -679,19 +679,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>138.16635</v>
+        <v>221.5</v>
       </c>
       <c r="C11" t="n">
-        <v>182.217146973062</v>
+        <v>174.8941768640577</v>
       </c>
       <c r="D11" t="n">
         <v>2.5</v>
       </c>
       <c r="E11" t="n">
-        <v>2832.043502651045</v>
+        <v>2817.006492904334</v>
       </c>
       <c r="F11" t="n">
-        <v>7.323045272477203</v>
+        <v>7.289754939244287</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -709,19 +709,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>132.156113775</v>
+        <v>215.5195</v>
       </c>
       <c r="C12" t="n">
-        <v>182.217146973062</v>
+        <v>174.8941768640577</v>
       </c>
       <c r="D12" t="n">
         <v>2.5</v>
       </c>
       <c r="E12" t="n">
-        <v>2832.043502651045</v>
+        <v>2817.006492904334</v>
       </c>
       <c r="F12" t="n">
-        <v>7.323045272477203</v>
+        <v>7.289754939244287</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -739,7 +739,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>140.00526015</v>
+        <v>225.01</v>
       </c>
       <c r="C13" t="n">
         <v>127.4114064737958</v>
@@ -748,10 +748,10 @@
         <v>2.5</v>
       </c>
       <c r="E13" t="n">
-        <v>2683.034274047157</v>
+        <v>2705.536401551786</v>
       </c>
       <c r="F13" t="n">
-        <v>6.968928334272836</v>
+        <v>7.025104808443722</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>98.46615966701712</v>
+        <v>99.49782569949188</v>
       </c>
     </row>
     <row r="14">
@@ -767,7 +767,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>140.00526015</v>
+        <v>225.01</v>
       </c>
       <c r="C14" t="n">
         <v>90</v>
@@ -797,19 +797,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>6.010236224999999</v>
+        <v>5.9805</v>
       </c>
       <c r="C15" t="n">
-        <v>182.217146973062</v>
+        <v>174.8941768640577</v>
       </c>
       <c r="D15" t="n">
         <v>2.5</v>
       </c>
       <c r="E15" t="n">
-        <v>2832.043502651045</v>
+        <v>2817.006492904334</v>
       </c>
       <c r="F15" t="n">
-        <v>7.323045272477203</v>
+        <v>7.289754939244287</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -827,19 +827,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>254.45</v>
+        <v>250</v>
       </c>
       <c r="C16" t="n">
-        <v>83.21022094302083</v>
+        <v>100.1968001138945</v>
       </c>
       <c r="D16" t="n">
         <v>2.5</v>
       </c>
       <c r="E16" t="n">
-        <v>348.6490395056206</v>
+        <v>420.1073802389807</v>
       </c>
       <c r="F16" t="n">
-        <v>1.113430167482677</v>
+        <v>1.309317439218598</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -857,19 +857,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>254.45</v>
+        <v>250</v>
       </c>
       <c r="C17" t="n">
-        <v>84.0846725437525</v>
+        <v>100.4932876541408</v>
       </c>
       <c r="D17" t="n">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E17" t="n">
-        <v>357.2416041823697</v>
+        <v>422.8205825802663</v>
       </c>
       <c r="F17" t="n">
-        <v>1.11947168026133</v>
+        <v>1.311135522056935</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>

</xml_diff>